<commit_message>
spending now prints plat saved before asking for plat left after
</commit_message>
<xml_diff>
--- a/lyr.xlsx
+++ b/lyr.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11835" windowWidth="21600" xWindow="825" yWindow="510"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="6450" yWindow="1635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -181,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -192,10 +192,8 @@
     <xf borderId="2" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="5" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="6" fillId="2" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="9" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -522,55 +520,55 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="11" width="9"/>
-    <col customWidth="1" max="4" min="4" style="26" width="28.5"/>
-    <col customWidth="1" max="7" min="7" style="26" width="9"/>
+    <col customWidth="1" max="3" min="1" style="10" width="9"/>
+    <col customWidth="1" max="4" min="4" style="24" width="28.5"/>
+    <col customWidth="1" max="7" min="7" style="24" width="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="n">
+      <c r="A1" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25" t="n">
+      <c r="B1" s="10" t="n">
+        <v>330454</v>
+      </c>
+      <c r="C1" s="23" t="n">
         <v>150000</v>
       </c>
-      <c r="D1" s="24" t="inlineStr">
+      <c r="D1" s="22" t="inlineStr">
         <is>
           <t>Current plat</t>
         </is>
       </c>
       <c r="E1" s="6" t="n">
-        <v>195896</v>
+        <v>230679</v>
       </c>
       <c r="G1" s="5" t="n">
         <v>43506</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
-        <v>330454</v>
-      </c>
-      <c r="B2" s="11" t="n">
+      <c r="A2" s="10" t="n">
         <v>261857</v>
       </c>
-      <c r="C2" s="11" t="n">
+      <c r="B2" s="25" t="n">
+        <v>261867</v>
+      </c>
+      <c r="C2" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="D2" s="14" t="inlineStr">
+      <c r="D2" s="12" t="inlineStr">
         <is>
           <t>Last plat</t>
         </is>
       </c>
-      <c r="E2" s="15" t="n">
-        <v>195896</v>
+      <c r="E2" s="13" t="n">
+        <v>230679</v>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
@@ -592,7 +590,7 @@
           <t>Kills</t>
         </is>
       </c>
-      <c r="K2" s="19" t="inlineStr">
+      <c r="K2" s="17" t="inlineStr">
         <is>
           <t>+Kills</t>
         </is>
@@ -602,7 +600,7 @@
           <t>Stats</t>
         </is>
       </c>
-      <c r="M2" s="19" t="inlineStr">
+      <c r="M2" s="17" t="inlineStr">
         <is>
           <t>+Stats</t>
         </is>
@@ -624,22 +622,22 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="27" t="n">
-        <v>261867</v>
-      </c>
-      <c r="B3" s="11" t="n">
+      <c r="A3" s="10" t="n">
         <v>202122</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="B3" s="25" t="n">
+        <v>231980</v>
+      </c>
+      <c r="C3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="inlineStr">
+      <c r="D3" s="12" t="inlineStr">
         <is>
           <t>Spending target</t>
         </is>
       </c>
-      <c r="E3" s="15" t="n">
-        <v>15000</v>
+      <c r="E3" s="13" t="n">
+        <v>10000</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0.03252314814814815</v>
@@ -667,21 +665,21 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="27" t="n">
+      <c r="A4" t="n">
         <v>231980</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="25" t="n">
         <v>231980</v>
       </c>
       <c r="C4" t="n">
         <v>2985</v>
       </c>
-      <c r="D4" s="14" t="inlineStr">
+      <c r="D4" s="12" t="inlineStr">
         <is>
           <t>Gain per kill</t>
         </is>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="20" t="n">
         <v>32.15</v>
       </c>
       <c r="G4" s="2" t="n">
@@ -719,11 +717,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="27" t="n">
-        <v>231980</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="A5" t="n">
         <v>174763</v>
+      </c>
+      <c r="B5" s="25" t="n">
+        <v>330168</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -733,7 +731,7 @@
           <t>Total saved</t>
         </is>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="21">
         <f>SUM(C:C)</f>
         <v/>
       </c>
@@ -770,10 +768,10 @@
       <c r="V5" s="8" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="27" t="n">
-        <v>330168</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="A6" t="n">
+        <v>190254</v>
+      </c>
+      <c r="B6" s="25" t="n">
         <v>190254</v>
       </c>
       <c r="C6" t="n">
@@ -808,11 +806,11 @@
       <c r="V6" s="8" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="27" t="n">
-        <v>190254</v>
-      </c>
-      <c r="B7" t="n">
+      <c r="A7" t="n">
         <v>175284</v>
+      </c>
+      <c r="B7" s="25" t="n">
+        <v>207964</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -846,11 +844,11 @@
       <c r="V7" s="8" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="27" t="n">
-        <v>207964</v>
-      </c>
-      <c r="B8" t="n">
+      <c r="A8" t="n">
         <v>189126</v>
+      </c>
+      <c r="B8" s="25" t="n">
+        <v>189131</v>
       </c>
       <c r="C8" t="n">
         <v>3268</v>
@@ -884,11 +882,11 @@
       <c r="V8" s="8" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="27" t="n">
-        <v>189131</v>
-      </c>
-      <c r="B9" t="n">
+      <c r="A9" t="n">
         <v>182570</v>
+      </c>
+      <c r="B9" s="25" t="n">
+        <v>203177</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -922,16 +920,16 @@
       <c r="V9" s="8" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="27" t="n">
-        <v>203177</v>
-      </c>
-      <c r="B10" t="n">
+      <c r="A10" t="n">
         <v>177944</v>
+      </c>
+      <c r="B10" s="25" t="n">
+        <v>220325</v>
       </c>
       <c r="C10" t="n">
         <v>2060</v>
       </c>
-      <c r="D10" s="12" t="n"/>
+      <c r="D10" s="11" t="n"/>
       <c r="G10" s="2" t="n">
         <v>0.7441319444444444</v>
       </c>
@@ -961,16 +959,16 @@
       <c r="V10" s="8" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="27" t="n">
-        <v>220325</v>
-      </c>
-      <c r="B11" t="n">
+      <c r="A11" t="n">
         <v>183797</v>
+      </c>
+      <c r="B11" s="25" t="n">
+        <v>239569</v>
       </c>
       <c r="C11" t="n">
         <v>4238</v>
       </c>
-      <c r="D11" s="12" t="n"/>
+      <c r="D11" s="11" t="n"/>
       <c r="G11" s="2" t="n"/>
       <c r="H11" s="1" t="n"/>
       <c r="I11" s="1">
@@ -992,16 +990,16 @@
       <c r="V11" s="8" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="27" t="n">
-        <v>239569</v>
-      </c>
-      <c r="B12" t="n">
+      <c r="A12" t="n">
         <v>212901</v>
+      </c>
+      <c r="B12" s="25" t="n">
+        <v>232366</v>
       </c>
       <c r="C12" t="n">
         <v>5577</v>
       </c>
-      <c r="D12" s="12" t="n"/>
+      <c r="D12" s="11" t="n"/>
       <c r="G12" s="2" t="n"/>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1">
@@ -1023,16 +1021,16 @@
       <c r="V12" s="8" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="27" t="n">
-        <v>232366</v>
-      </c>
-      <c r="B13" t="n">
+      <c r="A13" t="n">
         <v>187968</v>
+      </c>
+      <c r="B13" s="25" t="n">
+        <v>227918</v>
       </c>
       <c r="C13" t="n">
         <v>1946</v>
       </c>
-      <c r="D13" s="12" t="n"/>
+      <c r="D13" s="11" t="n"/>
       <c r="G13" s="2" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1">
@@ -1054,16 +1052,16 @@
       <c r="V13" s="8" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="n">
-        <v>227918</v>
-      </c>
-      <c r="B14" t="n">
+      <c r="A14" t="n">
         <v>188286</v>
+      </c>
+      <c r="B14" s="25" t="n">
+        <v>232161</v>
       </c>
       <c r="C14" t="n">
         <v>4997</v>
       </c>
-      <c r="D14" s="12" t="n"/>
+      <c r="D14" s="11" t="n"/>
       <c r="G14" s="2" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1">
@@ -1085,16 +1083,16 @@
       <c r="V14" s="8" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="27" t="n">
-        <v>232161</v>
-      </c>
-      <c r="B15" t="n">
+      <c r="A15" t="n">
         <v>202600</v>
+      </c>
+      <c r="B15" s="25" t="n">
+        <v>211125</v>
       </c>
       <c r="C15" t="n">
         <v>4387</v>
       </c>
-      <c r="D15" s="12" t="n"/>
+      <c r="D15" s="11" t="n"/>
       <c r="G15" s="2" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1">
@@ -1116,16 +1114,16 @@
       <c r="V15" s="8" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="27" t="n">
-        <v>211125</v>
-      </c>
-      <c r="B16" t="n">
+      <c r="A16" t="n">
         <v>202132</v>
+      </c>
+      <c r="B16" s="25" t="n">
+        <v>202134</v>
       </c>
       <c r="C16" t="n">
         <v>852</v>
       </c>
-      <c r="D16" s="12" t="n"/>
+      <c r="D16" s="11" t="n"/>
       <c r="G16" s="2" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1">
@@ -1147,16 +1145,16 @@
       <c r="V16" s="8" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="27" t="n">
-        <v>202134</v>
+      <c r="A17" t="n">
+        <v>195896</v>
       </c>
       <c r="B17" t="n">
-        <v>195896</v>
+        <v>244572</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="12" t="n"/>
+        <v>4867</v>
+      </c>
+      <c r="D17" s="11" t="n"/>
       <c r="G17" s="2" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1">
@@ -1178,8 +1176,10 @@
       <c r="V17" s="8" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="27" t="n"/>
-      <c r="D18" s="12" t="n"/>
+      <c r="A18" t="n">
+        <v>230662</v>
+      </c>
+      <c r="D18" s="11" t="n"/>
       <c r="G18" s="2" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1">
@@ -1201,8 +1201,8 @@
       <c r="V18" s="8" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="27" t="n"/>
-      <c r="D19" s="12" t="n"/>
+      <c r="A19" s="25" t="n"/>
+      <c r="D19" s="11" t="n"/>
       <c r="G19" s="2" t="n"/>
       <c r="H19" s="1" t="n"/>
       <c r="I19" s="1">
@@ -1224,8 +1224,8 @@
       <c r="V19" s="8" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="27" t="n"/>
-      <c r="D20" s="12" t="n"/>
+      <c r="A20" s="25" t="n"/>
+      <c r="D20" s="11" t="n"/>
       <c r="G20" s="2" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1">
@@ -1247,8 +1247,8 @@
       <c r="V20" s="8" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="n"/>
-      <c r="D21" s="12" t="n"/>
+      <c r="A21" s="25" t="n"/>
+      <c r="D21" s="11" t="n"/>
       <c r="G21" s="2" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1">
@@ -1270,7 +1270,7 @@
       <c r="V21" s="8" t="n"/>
     </row>
     <row r="22">
-      <c r="D22" s="12" t="n"/>
+      <c r="D22" s="11" t="n"/>
       <c r="G22" s="2" t="n"/>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1">
@@ -1292,7 +1292,7 @@
       <c r="V22" s="8" t="n"/>
     </row>
     <row r="23">
-      <c r="D23" s="12" t="n"/>
+      <c r="D23" s="11" t="n"/>
       <c r="G23" s="2" t="n"/>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1">
@@ -1314,23 +1314,23 @@
       <c r="V23" s="8" t="n"/>
     </row>
     <row r="24">
-      <c r="E24" s="11" t="n"/>
-      <c r="G24" s="20" t="n"/>
-      <c r="H24" s="17" t="inlineStr">
+      <c r="E24" s="10" t="n"/>
+      <c r="G24" s="18" t="n"/>
+      <c r="H24" s="15" t="inlineStr">
         <is>
           <t>Avg</t>
         </is>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="14">
         <f>AVERAGEIF(I4:I23,"&lt;&gt;0")</f>
         <v/>
       </c>
-      <c r="J24" s="18" t="n"/>
+      <c r="J24" s="16" t="n"/>
       <c r="K24" s="3">
         <f>AVERAGEIF(K4:K23,"&lt;&gt;0")</f>
         <v/>
       </c>
-      <c r="L24" s="18" t="n"/>
+      <c r="L24" s="16" t="n"/>
       <c r="M24" s="3">
         <f>AVERAGEIF(M4:M23,"&lt;&gt;0")</f>
         <v/>
@@ -1350,25 +1350,25 @@
       </c>
     </row>
     <row r="25">
-      <c r="G25" s="21" t="n"/>
+      <c r="G25" s="19" t="n"/>
     </row>
     <row r="26">
-      <c r="G26" s="21" t="n"/>
+      <c r="G26" s="19" t="n"/>
     </row>
     <row r="27">
-      <c r="G27" s="21" t="n"/>
+      <c r="G27" s="19" t="n"/>
     </row>
     <row r="28">
-      <c r="G28" s="21" t="n"/>
+      <c r="G28" s="19" t="n"/>
     </row>
     <row r="29">
-      <c r="G29" s="21" t="n"/>
+      <c r="G29" s="19" t="n"/>
     </row>
     <row r="30">
-      <c r="G30" s="21" t="n"/>
+      <c r="G30" s="19" t="n"/>
     </row>
     <row r="31">
-      <c r="G31" s="21" t="n"/>
+      <c r="G31" s="19" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Setup will now save path to a text file that python scripts will use to determine directory.
Arguably, this change wasn't needed but was a good learning experience.
</commit_message>
<xml_diff>
--- a/lyr.xlsx
+++ b/lyr.xlsx
@@ -3,19 +3,24 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="32190" yWindow="1530"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="6450" yWindow="1635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="4">
+    <numFmt formatCode="mmm&quot; &quot;d" numFmtId="164"/>
+    <numFmt formatCode="0&quot;p&quot;" numFmtId="165"/>
+    <numFmt formatCode="&quot;$&quot;#,##0.00" numFmtId="166"/>
+    <numFmt formatCode="0.0000&quot;g&quot;" numFmtId="167"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -25,28 +30,191 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="2" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="3" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -370,19 +538,12 @@
           <t>0</t>
         </is>
       </c>
-      <c r="B1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C1" t="n">
-        <v>1000</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1000</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
added spendingtargetcalc function to update option
note: maybe add lyr.xlsx to gitignore but leaving it out for now because im using that sheet to keep track of my own money
</commit_message>
<xml_diff>
--- a/lyr.xlsx
+++ b/lyr.xlsx
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,10 +547,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E3" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" t="n">
+        <v>52.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed prompts to write in next open cell
</commit_message>
<xml_diff>
--- a/lyr.xlsx
+++ b/lyr.xlsx
@@ -1,33 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LyrSave\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765D6F56-53D8-4FF3-831F-3772B135F471}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="28680" yWindow="-120"/>
+    <workbookView xWindow="30855" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>0</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -43,15 +56,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -339,61 +361,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>3000000</v>
       </c>
-      <c r="C1" t="n">
+      <c r="C1">
         <v>300000</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>348818</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>348842</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>4884</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
+        <v>360860</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>306781</v>
+      </c>
+      <c r="B3">
+        <v>414299</v>
+      </c>
+      <c r="C3">
+        <v>10751</v>
+      </c>
+      <c r="E3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>354611</v>
       </c>
+      <c r="B4">
+        <v>425621</v>
+      </c>
+      <c r="C4">
+        <v>7101</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>306781</v>
-      </c>
-      <c r="B3" t="n">
-        <v>414299</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10751</v>
-      </c>
-      <c r="E3" t="n">
-        <v>40000</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>360860</v>
+      </c>
+      <c r="B5">
+        <v>426032</v>
+      </c>
+      <c r="C5">
+        <v>6517</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>